<commit_message>
changed the employee table input
</commit_message>
<xml_diff>
--- a/Data_files/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Rotterdam_car_adjacency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD418AD2-C69E-4D7A-8B48-C01481F78521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC595D3-CF12-43A2-B218-15BC187939D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="860" windowWidth="19170" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection sqref="A1:T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1791,21 +1791,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -1949,10 +1934,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1974,19 +1984,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
lots of bugfixing and restoring the officeless adjacency graphs 2
</commit_message>
<xml_diff>
--- a/Data_files/Rotterdam_car_adjacency.xlsx
+++ b/Data_files/Rotterdam_car_adjacency.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB2550C-0543-4ADA-B842-5430B5FB4AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC3EC05-E381-4403-89B5-4DA99DDA7187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19170" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="R2" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="18">
         <v>1</v>
@@ -1504,7 +1504,7 @@
         <v>80.664968396488433</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -1791,21 +1791,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -1949,10 +1934,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1974,19 +1984,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>